<commit_message>
add full days_ahead and hold_thresh
</commit_message>
<xml_diff>
--- a/data/report_df/irs.xlsx
+++ b/data/report_df/irs.xlsx
@@ -366,7 +366,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -530,6 +530,167 @@
         <v>1.021269623304751</v>
       </c>
     </row>
+    <row r="8" spans="1:7">
+      <c r="A8" s="1">
+        <v>8</v>
+      </c>
+      <c r="B8">
+        <v>0.7489285731928166</v>
+      </c>
+      <c r="C8">
+        <v>0.8279462115860953</v>
+      </c>
+      <c r="D8">
+        <v>0.8055372423794177</v>
+      </c>
+      <c r="E8">
+        <v>0.9906730972243635</v>
+      </c>
+      <c r="F8">
+        <v>1.197432579484514</v>
+      </c>
+      <c r="G8">
+        <v>0.7602408221395534</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" s="1">
+        <v>9</v>
+      </c>
+      <c r="B9">
+        <v>1.10010523950836</v>
+      </c>
+      <c r="C9">
+        <v>1.12279591879383</v>
+      </c>
+      <c r="D9">
+        <v>1.537163856773588</v>
+      </c>
+      <c r="E9">
+        <v>1.264524664494019</v>
+      </c>
+      <c r="F9">
+        <v>1.1351442256939</v>
+      </c>
+      <c r="G9">
+        <v>0.946760951598782</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" s="1">
+        <v>10</v>
+      </c>
+      <c r="B10">
+        <v>0.8231969701403786</v>
+      </c>
+      <c r="C10">
+        <v>1.164292629627047</v>
+      </c>
+      <c r="D10">
+        <v>1.063463882421663</v>
+      </c>
+      <c r="E10">
+        <v>1.101371799224184</v>
+      </c>
+      <c r="F10">
+        <v>1.301639401483388</v>
+      </c>
+      <c r="G10">
+        <v>1.06516361803197</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" s="1">
+        <v>11</v>
+      </c>
+      <c r="B11">
+        <v>0.7308399557844771</v>
+      </c>
+      <c r="C11">
+        <v>0.6789794128506424</v>
+      </c>
+      <c r="D11">
+        <v>0.6116870057193515</v>
+      </c>
+      <c r="E11">
+        <v>0.6490724813146383</v>
+      </c>
+      <c r="F11">
+        <v>0.9481986454493596</v>
+      </c>
+      <c r="G11">
+        <v>1.234403594205529</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12" s="1">
+        <v>12</v>
+      </c>
+      <c r="B12">
+        <v>0.9303135594904726</v>
+      </c>
+      <c r="C12">
+        <v>1.174207595199213</v>
+      </c>
+      <c r="D12">
+        <v>0.9822517680118442</v>
+      </c>
+      <c r="E12">
+        <v>1.135300177435434</v>
+      </c>
+      <c r="F12">
+        <v>1.281085910869446</v>
+      </c>
+      <c r="G12">
+        <v>1.341625807083262</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13" s="1">
+        <v>13</v>
+      </c>
+      <c r="B13">
+        <v>0.898281320836375</v>
+      </c>
+      <c r="C13">
+        <v>0.8523280122664625</v>
+      </c>
+      <c r="D13">
+        <v>1.147700678224136</v>
+      </c>
+      <c r="E13">
+        <v>1.050865029082537</v>
+      </c>
+      <c r="F13">
+        <v>1.142395796240432</v>
+      </c>
+      <c r="G13">
+        <v>1.074238764262095</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14" s="1">
+        <v>14</v>
+      </c>
+      <c r="B14">
+        <v>1.264939569612696</v>
+      </c>
+      <c r="C14">
+        <v>1.11724155029655</v>
+      </c>
+      <c r="D14">
+        <v>1.081276692631159</v>
+      </c>
+      <c r="E14">
+        <v>1.443104718815984</v>
+      </c>
+      <c r="F14">
+        <v>1.382728978810254</v>
+      </c>
+      <c r="G14">
+        <v>1.360412685622154</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>